<commit_message>
Fixed health calculating formula in excel file. Precalculated base health values with the 0.9 multiplier.
</commit_message>
<xml_diff>
--- a/Research/DataMining.xlsx
+++ b/Research/DataMining.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,8 +513,8 @@
         <v>4</v>
       </c>
       <c r="G10" s="5">
-        <f ca="1">ROUNDUP((ROUNDUP(0.9*B4,0)+10*ROUNDUP(B5*B11,0))*B15,0)</f>
-        <v>7470</v>
+        <f ca="1">ROUND((ROUND(0.9*B4 - 0.01,0)+10*ROUND(B5*B11 - 0.01,0))*B15 - 0.01,0)</f>
+        <v>15774</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -562,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>0.37990000000000002</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +644,10 @@
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2">
+        <f>ROUND(B2*0.9 - 0.01, 0)</f>
+        <v>0</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2">
         <v>5</v>
@@ -661,6 +665,10 @@
       <c r="B3">
         <v>20</v>
       </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">ROUND(B3*0.9 - 0.01, 0)</f>
+        <v>18</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3">
         <v>10</v>
@@ -678,6 +686,10 @@
       <c r="B4">
         <v>40</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4">
         <v>17</v>
@@ -695,6 +707,10 @@
       <c r="B5">
         <v>60</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5">
         <v>22</v>
@@ -712,6 +728,10 @@
       <c r="B6">
         <v>80</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6">
         <v>27</v>
@@ -729,6 +749,10 @@
       <c r="B7">
         <v>100</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7">
         <v>35</v>
@@ -746,6 +770,10 @@
       <c r="B8">
         <v>120</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8">
         <v>45</v>
@@ -763,6 +791,10 @@
       <c r="B9">
         <v>140</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9">
         <v>50</v>
@@ -780,6 +812,10 @@
       <c r="B10">
         <v>160</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10">
         <v>55</v>
@@ -797,6 +833,10 @@
       <c r="B11">
         <v>180</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11">
         <v>60</v>
@@ -814,6 +854,10 @@
       <c r="B12">
         <v>200</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12">
         <v>68</v>
@@ -831,6 +875,10 @@
       <c r="B13">
         <v>220</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13">
         <v>76</v>
@@ -848,6 +896,10 @@
       <c r="B14">
         <v>240</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14">
         <v>84</v>
@@ -865,6 +917,10 @@
       <c r="B15">
         <v>260</v>
       </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>234</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15">
         <v>92</v>
@@ -882,6 +938,10 @@
       <c r="B16">
         <v>265</v>
       </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>238</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16">
         <v>94</v>
@@ -899,6 +959,10 @@
       <c r="B17">
         <v>270</v>
       </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17">
         <v>95</v>
@@ -916,6 +980,10 @@
       <c r="B18">
         <v>292</v>
       </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>263</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18">
         <v>103</v>
@@ -933,6 +1001,10 @@
       <c r="B19">
         <v>306</v>
       </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19">
         <v>108</v>
@@ -950,6 +1022,10 @@
       <c r="B20">
         <v>319</v>
       </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>287</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20">
         <v>112</v>
@@ -967,6 +1043,10 @@
       <c r="B21">
         <v>332</v>
       </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>299</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21">
         <v>116</v>
@@ -984,6 +1064,10 @@
       <c r="B22">
         <v>370</v>
       </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>333</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22">
         <v>123</v>
@@ -1001,6 +1085,10 @@
       <c r="B23">
         <v>408</v>
       </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>367</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23">
         <v>129</v>
@@ -1018,6 +1106,10 @@
       <c r="B24">
         <v>462</v>
       </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>416</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24">
         <v>140</v>
@@ -1035,6 +1127,10 @@
       <c r="B25">
         <v>501</v>
       </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>451</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25">
         <v>147</v>
@@ -1052,6 +1148,10 @@
       <c r="B26">
         <v>538</v>
       </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>484</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26">
         <v>153</v>
@@ -1069,6 +1169,10 @@
       <c r="B27">
         <v>575</v>
       </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27">
         <v>160</v>
@@ -1086,6 +1190,10 @@
       <c r="B28">
         <v>611</v>
       </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28">
         <v>166</v>
@@ -1103,6 +1211,10 @@
       <c r="B29">
         <v>646</v>
       </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>581</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29">
         <v>171</v>
@@ -1120,6 +1232,10 @@
       <c r="B30">
         <v>713</v>
       </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>642</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30">
         <v>186</v>
@@ -1137,6 +1253,10 @@
       <c r="B31">
         <v>750</v>
       </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>675</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31">
         <v>192</v>
@@ -1154,6 +1274,10 @@
       <c r="B32">
         <v>818</v>
       </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>736</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32">
         <v>208</v>
@@ -1171,6 +1295,10 @@
       <c r="B33">
         <v>855</v>
       </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>769</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33">
         <v>219</v>
@@ -1188,6 +1316,10 @@
       <c r="B34">
         <v>892</v>
       </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>803</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34">
         <v>230</v>
@@ -1205,6 +1337,10 @@
       <c r="B35">
         <v>928</v>
       </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>835</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35">
         <v>238</v>
@@ -1222,6 +1358,10 @@
       <c r="B36">
         <v>995</v>
       </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>895</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36">
         <v>253</v>
@@ -1239,6 +1379,10 @@
       <c r="B37">
         <v>1032</v>
       </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>929</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37">
         <v>259</v>
@@ -1256,6 +1400,10 @@
       <c r="B38">
         <v>1103</v>
       </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>993</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38">
         <v>274</v>
@@ -1273,6 +1421,10 @@
       <c r="B39">
         <v>1141</v>
       </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1027</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39">
         <v>279</v>
@@ -1290,6 +1442,10 @@
       <c r="B40">
         <v>1178</v>
       </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>1060</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40">
         <v>284</v>
@@ -1307,6 +1463,10 @@
       <c r="B41">
         <v>1215</v>
       </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>1093</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41">
         <v>290</v>
@@ -1324,6 +1484,10 @@
       <c r="B42">
         <v>1328</v>
       </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>1195</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42">
         <v>304</v>
@@ -1341,6 +1505,10 @@
       <c r="B43">
         <v>1410</v>
       </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>1269</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43">
         <v>317</v>
@@ -1358,6 +1526,10 @@
       <c r="B44">
         <v>1531</v>
       </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>1378</v>
+      </c>
       <c r="D44" s="1"/>
       <c r="E44">
         <v>339</v>
@@ -1375,6 +1547,10 @@
       <c r="B45">
         <v>1614</v>
       </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>1453</v>
+      </c>
       <c r="D45" s="1"/>
       <c r="E45">
         <v>353</v>
@@ -1392,6 +1568,10 @@
       <c r="B46">
         <v>1695</v>
       </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>1525</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46">
         <v>366</v>
@@ -1409,6 +1589,10 @@
       <c r="B47">
         <v>1776</v>
       </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>1598</v>
+      </c>
       <c r="D47" s="1"/>
       <c r="E47">
         <v>380</v>
@@ -1426,6 +1610,10 @@
       <c r="B48">
         <v>1892</v>
       </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>1703</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48">
         <v>401</v>
@@ -1443,6 +1631,10 @@
       <c r="B49">
         <v>1974</v>
       </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>1777</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49">
         <v>416</v>
@@ -1460,6 +1652,10 @@
       <c r="B50">
         <v>2101</v>
       </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>1891</v>
+      </c>
       <c r="D50" s="1"/>
       <c r="E50">
         <v>440</v>
@@ -1477,6 +1673,10 @@
       <c r="B51">
         <v>2183</v>
       </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>1965</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51">
         <v>454</v>
@@ -1494,6 +1694,10 @@
       <c r="B52">
         <v>2265</v>
       </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52">
         <v>471</v>
@@ -1511,6 +1715,10 @@
       <c r="B53">
         <v>2346</v>
       </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>2111</v>
+      </c>
       <c r="D53" s="1"/>
       <c r="E53">
         <v>488</v>
@@ -1528,6 +1736,10 @@
       <c r="B54">
         <v>2464</v>
       </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>2218</v>
+      </c>
       <c r="D54" s="1"/>
       <c r="E54">
         <v>514</v>
@@ -1545,6 +1757,10 @@
       <c r="B55">
         <v>2547</v>
       </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>2292</v>
+      </c>
       <c r="D55" s="1"/>
       <c r="E55">
         <v>532</v>
@@ -1562,6 +1778,10 @@
       <c r="B56">
         <v>2677</v>
       </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>2409</v>
+      </c>
       <c r="D56" s="1"/>
       <c r="E56">
         <v>561</v>
@@ -1579,6 +1799,10 @@
       <c r="B57">
         <v>2760</v>
       </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>2484</v>
+      </c>
       <c r="D57" s="1"/>
       <c r="E57">
         <v>579</v>
@@ -1596,6 +1820,10 @@
       <c r="B58">
         <v>2842</v>
       </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>2558</v>
+      </c>
       <c r="D58" s="1"/>
       <c r="E58">
         <v>598</v>
@@ -1613,6 +1841,10 @@
       <c r="B59">
         <v>2924</v>
       </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>2632</v>
+      </c>
       <c r="D59" s="1"/>
       <c r="E59">
         <v>617</v>
@@ -1630,6 +1862,10 @@
       <c r="B60">
         <v>3040</v>
       </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>2736</v>
+      </c>
       <c r="D60" s="1"/>
       <c r="E60">
         <v>643</v>
@@ -1647,6 +1883,10 @@
       <c r="B61">
         <v>3122</v>
       </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>2810</v>
+      </c>
       <c r="D61" s="1"/>
       <c r="E61">
         <v>662</v>
@@ -1664,6 +1904,10 @@
       <c r="B62">
         <v>3303</v>
       </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>2973</v>
+      </c>
       <c r="D62" s="1"/>
       <c r="E62">
         <v>696</v>
@@ -1681,6 +1925,10 @@
       <c r="B63">
         <v>3432</v>
       </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>3089</v>
+      </c>
       <c r="D63" s="1"/>
       <c r="E63">
         <v>718</v>
@@ -1698,6 +1946,10 @@
       <c r="B64">
         <v>3561</v>
       </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>3205</v>
+      </c>
       <c r="D64" s="1"/>
       <c r="E64">
         <v>741</v>
@@ -1715,6 +1967,10 @@
       <c r="B65">
         <v>3688</v>
       </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>3319</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65">
         <v>765</v>
@@ -1732,6 +1988,10 @@
       <c r="B66">
         <v>3852</v>
       </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>3467</v>
+      </c>
       <c r="D66" s="1"/>
       <c r="E66">
         <v>795</v>
@@ -1749,6 +2009,10 @@
       <c r="B67">
         <v>3980</v>
       </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C102" si="1">ROUND(B67*0.9 - 0.01, 0)</f>
+        <v>3582</v>
+      </c>
       <c r="D67" s="1"/>
       <c r="E67">
         <v>818</v>
@@ -1766,6 +2030,10 @@
       <c r="B68">
         <v>4226</v>
       </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>3803</v>
+      </c>
       <c r="D68" s="1"/>
       <c r="E68">
         <v>866</v>
@@ -1783,6 +2051,10 @@
       <c r="B69">
         <v>4357</v>
       </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>3921</v>
+      </c>
       <c r="D69" s="1"/>
       <c r="E69">
         <v>891</v>
@@ -1800,6 +2072,10 @@
       <c r="B70">
         <v>4487</v>
       </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>4038</v>
+      </c>
       <c r="D70" s="1"/>
       <c r="E70">
         <v>916</v>
@@ -1817,6 +2093,10 @@
       <c r="B71">
         <v>4616</v>
       </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>4154</v>
+      </c>
       <c r="D71" s="1"/>
       <c r="E71">
         <v>941</v>
@@ -1834,6 +2114,10 @@
       <c r="B72">
         <v>4774</v>
       </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>4297</v>
+      </c>
       <c r="D72" s="1"/>
       <c r="E72">
         <v>976</v>
@@ -1851,6 +2135,10 @@
       <c r="B73">
         <v>4904</v>
       </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>4414</v>
+      </c>
       <c r="D73" s="1"/>
       <c r="E73">
         <v>1004</v>
@@ -1868,6 +2156,10 @@
       <c r="B74">
         <v>5164</v>
       </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>4648</v>
+      </c>
       <c r="D74" s="1"/>
       <c r="E74">
         <v>1059</v>
@@ -1885,6 +2177,10 @@
       <c r="B75">
         <v>5295</v>
       </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>4765</v>
+      </c>
       <c r="D75" s="1"/>
       <c r="E75">
         <v>1089</v>
@@ -1902,6 +2198,10 @@
       <c r="B76">
         <v>5426</v>
       </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>4883</v>
+      </c>
       <c r="D76" s="1"/>
       <c r="E76">
         <v>1119</v>
@@ -1919,6 +2219,10 @@
       <c r="B77">
         <v>5557</v>
       </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>5001</v>
+      </c>
       <c r="D77" s="1"/>
       <c r="E77">
         <v>1149</v>
@@ -1936,6 +2240,10 @@
       <c r="B78">
         <v>5710</v>
       </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>5139</v>
+      </c>
       <c r="D78" s="1"/>
       <c r="E78">
         <v>1183</v>
@@ -1953,6 +2261,10 @@
       <c r="B79">
         <v>5841</v>
       </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>5257</v>
+      </c>
       <c r="D79" s="1"/>
       <c r="E79">
         <v>1214</v>
@@ -1970,6 +2282,10 @@
       <c r="B80">
         <v>6112</v>
       </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>5501</v>
+      </c>
       <c r="D80" s="1"/>
       <c r="E80">
         <v>1274</v>
@@ -1987,6 +2303,10 @@
       <c r="B81">
         <v>6245</v>
       </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>5620</v>
+      </c>
       <c r="D81" s="1"/>
       <c r="E81">
         <v>1307</v>
@@ -2004,6 +2324,10 @@
       <c r="B82">
         <v>6580</v>
       </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>5922</v>
+      </c>
       <c r="D82" s="1"/>
       <c r="E82">
         <v>1374</v>
@@ -2021,6 +2345,10 @@
       <c r="B83">
         <v>6780</v>
       </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>6102</v>
+      </c>
       <c r="D83" s="1"/>
       <c r="E83">
         <v>1413</v>
@@ -2038,6 +2366,10 @@
       <c r="B84">
         <v>6980</v>
       </c>
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>6282</v>
+      </c>
       <c r="D84" s="1"/>
       <c r="E84">
         <v>1453</v>
@@ -2055,6 +2387,10 @@
       <c r="B85">
         <v>7180</v>
       </c>
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>6462</v>
+      </c>
       <c r="D85" s="1"/>
       <c r="E85">
         <v>1493</v>
@@ -2072,6 +2408,10 @@
       <c r="B86">
         <v>7380</v>
       </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>6642</v>
+      </c>
       <c r="D86" s="1"/>
       <c r="E86">
         <v>1534</v>
@@ -2089,6 +2429,10 @@
       <c r="B87">
         <v>7580</v>
       </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>6822</v>
+      </c>
       <c r="D87" s="1"/>
       <c r="E87">
         <v>1575</v>
@@ -2106,6 +2450,10 @@
       <c r="B88">
         <v>7780</v>
       </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>7002</v>
+      </c>
       <c r="D88" s="1"/>
       <c r="E88">
         <v>1616</v>
@@ -2123,6 +2471,10 @@
       <c r="B89">
         <v>7980</v>
       </c>
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>7182</v>
+      </c>
       <c r="D89" s="1"/>
       <c r="E89">
         <v>1658</v>
@@ -2140,6 +2492,10 @@
       <c r="B90">
         <v>8180</v>
       </c>
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>7362</v>
+      </c>
       <c r="D90" s="1"/>
       <c r="E90">
         <v>1700</v>
@@ -2157,6 +2513,10 @@
       <c r="B91">
         <v>8380</v>
       </c>
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>7542</v>
+      </c>
       <c r="D91" s="1"/>
       <c r="E91">
         <v>1743</v>
@@ -2174,6 +2534,10 @@
       <c r="B92">
         <v>8580</v>
       </c>
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>7722</v>
+      </c>
       <c r="D92" s="1"/>
       <c r="E92">
         <v>1786</v>
@@ -2191,6 +2555,10 @@
       <c r="B93">
         <v>8780</v>
       </c>
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>7902</v>
+      </c>
       <c r="D93" s="1"/>
       <c r="E93">
         <v>1829</v>
@@ -2208,6 +2576,10 @@
       <c r="B94">
         <v>8980</v>
       </c>
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>8082</v>
+      </c>
       <c r="D94" s="1"/>
       <c r="E94">
         <v>1873</v>
@@ -2225,6 +2597,10 @@
       <c r="B95">
         <v>9180</v>
       </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>8262</v>
+      </c>
       <c r="D95" s="1"/>
       <c r="E95">
         <v>1917</v>
@@ -2242,6 +2618,10 @@
       <c r="B96">
         <v>9380</v>
       </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>8442</v>
+      </c>
       <c r="D96" s="1"/>
       <c r="E96">
         <v>1961</v>
@@ -2259,6 +2639,10 @@
       <c r="B97">
         <v>9580</v>
       </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>8622</v>
+      </c>
       <c r="D97" s="1"/>
       <c r="E97">
         <v>2006</v>
@@ -2276,6 +2660,10 @@
       <c r="B98">
         <v>9780</v>
       </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>8802</v>
+      </c>
       <c r="D98" s="1"/>
       <c r="E98">
         <v>2052</v>
@@ -2293,6 +2681,10 @@
       <c r="B99">
         <v>9980</v>
       </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>8982</v>
+      </c>
       <c r="D99" s="1"/>
       <c r="E99">
         <v>2098</v>
@@ -2310,6 +2702,10 @@
       <c r="B100">
         <v>10180</v>
       </c>
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>9162</v>
+      </c>
       <c r="D100" s="1"/>
       <c r="E100">
         <v>2144</v>
@@ -2327,6 +2723,10 @@
       <c r="B101">
         <v>10380</v>
       </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>9342</v>
+      </c>
       <c r="D101" s="1"/>
       <c r="E101">
         <v>2190</v>
@@ -2343,6 +2743,10 @@
       <c r="A102" s="1"/>
       <c r="B102">
         <v>10580</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>9522</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102">

</xml_diff>